<commit_message>
Fix MySQL DB connection and update server.py
</commit_message>
<xml_diff>
--- a/backend/users.xlsx
+++ b/backend/users.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -611,9 +611,69 @@
           <t>sadadss@gmail.com</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>9879808966</t>
+      <c r="F6" t="n">
+        <v>9879808966</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Pon Sankar</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2011-03-04</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>pon_sankar</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>ponsankar389@gmail.com</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>7890564567</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Ashwin</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2001-05-31</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>ashwin_389</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>ashwin389@gmail.com</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>8978788677</t>
         </is>
       </c>
     </row>

</xml_diff>